<commit_message>
"add ours column to punch data table"
</commit_message>
<xml_diff>
--- a/matlab_XLR.xlsx
+++ b/matlab_XLR.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amir/Documents/MATLAB/projects/personal/sturgeon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9D941-25C7-F949-AEC0-60EED276237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD16AA-EFCF-AB44-A535-30670DA0620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QGrLkjpZ/FrsaOvcAlUi3y0wqrbWO7AFW5zcSLoKSo4Nb9/O3Yu89zxtGFdXySWyKZJbJaecsHrwUFT1zxTdOw==" workbookSaltValue="Ss0wH5ugGyVcBuy9TWGm0g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26533" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26532" uniqueCount="1290">
   <si>
     <t>Results of Analysis   VA23B0556</t>
   </si>
@@ -6391,11 +6391,11 @@
   <sheetPr codeName="Results Summary"/>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6997,8 +6997,8 @@
       <c r="K10" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>500</v>
+      <c r="L10" s="9">
+        <v>0.93100000000000005</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>542</v>
@@ -73353,11 +73353,24 @@
   </sheetData>
   <autoFilter ref="A9:Q1250" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="35">
-    <mergeCell ref="A1036:D1036"/>
-    <mergeCell ref="A1106:D1106"/>
-    <mergeCell ref="A1109:D1109"/>
-    <mergeCell ref="A1179:D1179"/>
-    <mergeCell ref="A1182:D1182"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A595:D595"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A233:D233"/>
+    <mergeCell ref="A303:D303"/>
+    <mergeCell ref="A306:D306"/>
+    <mergeCell ref="A376:D376"/>
+    <mergeCell ref="A379:D379"/>
+    <mergeCell ref="A449:D449"/>
+    <mergeCell ref="A452:D452"/>
+    <mergeCell ref="A522:D522"/>
+    <mergeCell ref="A525:D525"/>
     <mergeCell ref="A1033:D1033"/>
     <mergeCell ref="A598:D598"/>
     <mergeCell ref="A668:D668"/>
@@ -73370,24 +73383,11 @@
     <mergeCell ref="A890:D890"/>
     <mergeCell ref="A960:D960"/>
     <mergeCell ref="A963:D963"/>
-    <mergeCell ref="A595:D595"/>
-    <mergeCell ref="A160:D160"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A233:D233"/>
-    <mergeCell ref="A303:D303"/>
-    <mergeCell ref="A306:D306"/>
-    <mergeCell ref="A376:D376"/>
-    <mergeCell ref="A379:D379"/>
-    <mergeCell ref="A449:D449"/>
-    <mergeCell ref="A452:D452"/>
-    <mergeCell ref="A522:D522"/>
-    <mergeCell ref="A525:D525"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A1036:D1036"/>
+    <mergeCell ref="A1106:D1106"/>
+    <mergeCell ref="A1109:D1109"/>
+    <mergeCell ref="A1179:D1179"/>
+    <mergeCell ref="A1182:D1182"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -73398,7 +73398,7 @@
   <sheetPr codeName="Duplicates"/>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q35"/>
     </sheetView>

</xml_diff>

<commit_message>
"punch_ours bar plot added"
</commit_message>
<xml_diff>
--- a/matlab_XLR.xlsx
+++ b/matlab_XLR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amir/Documents/MATLAB/projects/personal/sturgeon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD16AA-EFCF-AB44-A535-30670DA0620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18674CDC-33DD-AC4D-A4E5-A288B77FE5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QGrLkjpZ/FrsaOvcAlUi3y0wqrbWO7AFW5zcSLoKSo4Nb9/O3Yu89zxtGFdXySWyKZJbJaecsHrwUFT1zxTdOw==" workbookSaltValue="Ss0wH5ugGyVcBuy9TWGm0g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26532" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26533" uniqueCount="1290">
   <si>
     <t>Results of Analysis   VA23B0556</t>
   </si>
@@ -6392,10 +6392,10 @@
   <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6997,8 +6997,8 @@
       <c r="K10" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="L10" s="9">
-        <v>0.93100000000000005</v>
+      <c r="L10" s="9" t="s">
+        <v>500</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>542</v>

</xml_diff>